<commit_message>
Cleaning up spt100 data
</commit_message>
<xml_diff>
--- a/doc/spt100/spt100-datasets.xlsx
+++ b/doc/spt100/spt100-datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eckel\Documents\GitHub\HallThrusterPEM\doc\spt100\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CF2418-CB8D-44A0-913A-3C8342F289FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5316FD-8C86-4015-9E67-2D347CA8F2C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E5D0682F-4288-449C-90F8-0C78832D07D3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="8" xr2:uid="{E5D0682F-4288-449C-90F8-0C78832D07D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -1244,7 +1244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A102C5B-46CF-4937-B343-5EA983A5DF4B}">
   <dimension ref="C1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -9910,8 +9910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{594DA2F1-5E06-4B69-8761-B624FFCC9C9D}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>